<commit_message>
Add extraction main info from sheets
</commit_message>
<xml_diff>
--- a/data/Отметки_1.xlsx
+++ b/data/Отметки_1.xlsx
@@ -23,7 +23,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -42,7 +42,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -61,7 +61,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -80,7 +80,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -99,7 +99,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -115,7 +115,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -131,7 +131,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -147,7 +147,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -163,7 +163,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -179,7 +179,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -195,7 +195,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -211,7 +211,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -227,7 +227,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -243,7 +243,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -259,7 +259,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -275,7 +275,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -291,7 +291,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -307,7 +307,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -323,7 +323,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -339,7 +339,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -355,7 +355,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -371,7 +371,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -387,7 +387,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -403,7 +403,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -419,7 +419,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -435,7 +435,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -451,7 +451,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -467,7 +467,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -483,7 +483,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -499,7 +499,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -515,7 +515,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -531,7 +531,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -547,7 +547,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -563,7 +563,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -579,7 +579,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -595,7 +595,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -611,7 +611,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -627,7 +627,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -643,7 +643,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -659,7 +659,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -675,7 +675,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1196,7 +1196,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1210,7 +1210,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1221,6 +1221,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1255,12 +1261,12 @@
   <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1615,374 +1621,374 @@
     <col min="37" max="37" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1"/>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-      <c r="AK8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="2">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -2095,8 +2101,8 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A11" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2170,8 +2176,8 @@
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A12" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2237,8 +2243,8 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A13" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A13" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B13" s="3"/>
@@ -2292,8 +2298,8 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A14" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2359,8 +2365,8 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A15" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A15" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2432,8 +2438,8 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A16" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A16" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="3"/>
@@ -2511,8 +2517,8 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A17" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="3"/>
@@ -2564,8 +2570,8 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A18" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2641,8 +2647,8 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A19" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -2718,8 +2724,8 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A20" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A20" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -2773,8 +2779,8 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="31.5" customFormat="1" s="2">
-      <c r="A21" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="31.5" customFormat="1" s="1">
+      <c r="A21" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B21" s="3"/>
@@ -2826,8 +2832,8 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A22" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A22" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B22" s="3"/>
@@ -2901,8 +2907,8 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A23" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A23" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B23" s="3"/>
@@ -2952,8 +2958,8 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A24" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A24" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B24" s="3"/>
@@ -3017,8 +3023,8 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A25" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A25" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B25" s="3"/>
@@ -3084,8 +3090,8 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25" customFormat="1" s="2">
-      <c r="A26" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A26" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B26" s="3"/>
@@ -3149,85 +3155,85 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-      <c r="AE27" s="1"/>
-      <c r="AF27" s="1"/>
-      <c r="AG27" s="1"/>
-      <c r="AH27" s="1"/>
-      <c r="AI27" s="1"/>
-      <c r="AJ27" s="1"/>
-      <c r="AK27" s="1"/>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+      <c r="AJ27" s="2"/>
+      <c r="AK27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="48.75">
-      <c r="A28" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="48.75" customFormat="1" s="1">
+      <c r="A28" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="1"/>
-      <c r="AE28" s="1"/>
-      <c r="AF28" s="1"/>
-      <c r="AG28" s="1"/>
-      <c r="AH28" s="1"/>
-      <c r="AI28" s="1"/>
-      <c r="AJ28" s="1"/>
-      <c r="AK28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="2"/>
+      <c r="AK28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>